<commit_message>
update paper selection excel
</commit_message>
<xml_diff>
--- a/paper_selection/interface/paper_selection.xlsx
+++ b/paper_selection/interface/paper_selection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lfoppiano/development/projects/grobid/grobid-superconductors/resources/web/paper_selection/interface/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lfoppiano/development/projects/grobid/grobid-superconductors/resources/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{27E5B4FB-AF8A-0F4C-93CB-E548AEB7CB73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3EC0D5B8-DF55-5644-8C7E-E511AAE141A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="2560" windowWidth="27240" windowHeight="16440"/>
+    <workbookView xWindow="6360" yWindow="2560" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output" sheetId="1" r:id="rId1"/>
@@ -1596,8 +1596,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1728,6 +1728,14 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2030,7 +2038,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2073,12 +2081,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -2112,6 +2122,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2431,11 +2442,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2479,7 +2490,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR06015055-CC.pdf", "PR06015055-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR06015055-CC.pdf", "PR06015055-CC.pdf")</f>
         <v>PR06015055-CC.pdf</v>
       </c>
       <c r="C2" t="s">
@@ -2499,8 +2510,8 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR05003221-CC.pdf", "PR05003221-CC.pdf")</f>
+      <c r="B3" s="2" t="str">
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR05003221-CC.pdf", "PR05003221-CC.pdf")</f>
         <v>PR05003221-CC.pdf</v>
       </c>
       <c r="C3" t="s">
@@ -2521,7 +2532,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR05809504-CC.pdf", "PR05809504-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR05809504-CC.pdf", "PR05809504-CC.pdf")</f>
         <v>PR05809504-CC.pdf</v>
       </c>
       <c r="C4" t="s">
@@ -2542,7 +2553,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR05514733-CC.pdf", "PR05514733-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR05514733-CC.pdf", "PR05514733-CC.pdf")</f>
         <v>PR05514733-CC.pdf</v>
       </c>
       <c r="C5" t="s">
@@ -2563,7 +2574,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR05703245-CC.pdf", "PR05703245-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR05703245-CC.pdf", "PR05703245-CC.pdf")</f>
         <v>PR05703245-CC.pdf</v>
       </c>
       <c r="D6" t="s">
@@ -2581,7 +2592,7 @@
         <v>21</v>
       </c>
       <c r="B7" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR06103604-CC.pdf", "PR06103604-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR06103604-CC.pdf", "PR06103604-CC.pdf")</f>
         <v>PR06103604-CC.pdf</v>
       </c>
       <c r="C7" t="s">
@@ -2602,7 +2613,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR06100107-CC.pdf", "PR06100107-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR06100107-CC.pdf", "PR06100107-CC.pdf")</f>
         <v>PR06100107-CC.pdf</v>
       </c>
       <c r="C8" t="s">
@@ -2623,7 +2634,7 @@
         <v>27</v>
       </c>
       <c r="B9" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR05814581-CC.pdf", "PR05814581-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR05814581-CC.pdf", "PR05814581-CC.pdf")</f>
         <v>PR05814581-CC.pdf</v>
       </c>
       <c r="C9" t="s">
@@ -2644,7 +2655,7 @@
         <v>30</v>
       </c>
       <c r="B10" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR04909084-CC.pdf", "PR04909084-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR04909084-CC.pdf", "PR04909084-CC.pdf")</f>
         <v>PR04909084-CC.pdf</v>
       </c>
       <c r="C10" t="s">
@@ -2665,7 +2676,7 @@
         <v>33</v>
       </c>
       <c r="B11" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR06006991-CC.pdf", "PR06006991-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR06006991-CC.pdf", "PR06006991-CC.pdf")</f>
         <v>PR06006991-CC.pdf</v>
       </c>
       <c r="C11" t="s">
@@ -2686,7 +2697,7 @@
         <v>36</v>
       </c>
       <c r="B12" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR05903948-CC.pdf", "PR05903948-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR05903948-CC.pdf", "PR05903948-CC.pdf")</f>
         <v>PR05903948-CC.pdf</v>
       </c>
       <c r="C12" t="s">
@@ -2707,7 +2718,7 @@
         <v>39</v>
       </c>
       <c r="B13" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR06013094-CC.pdf", "PR06013094-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR06013094-CC.pdf", "PR06013094-CC.pdf")</f>
         <v>PR06013094-CC.pdf</v>
       </c>
       <c r="C13" t="s">
@@ -2728,7 +2739,7 @@
         <v>42</v>
       </c>
       <c r="B14" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR0446999-CC.pdf", "PR0446999-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR0446999-CC.pdf", "PR0446999-CC.pdf")</f>
         <v>PR0446999-CC.pdf</v>
       </c>
       <c r="D14" t="s">
@@ -2746,7 +2757,7 @@
         <v>44</v>
       </c>
       <c r="B15" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR04310568-CC.pdf", "PR04310568-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR04310568-CC.pdf", "PR04310568-CC.pdf")</f>
         <v>PR04310568-CC.pdf</v>
       </c>
       <c r="C15" t="s">
@@ -2767,7 +2778,7 @@
         <v>47</v>
       </c>
       <c r="B16" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR05914099-CC.pdf", "PR05914099-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR05914099-CC.pdf", "PR05914099-CC.pdf")</f>
         <v>PR05914099-CC.pdf</v>
       </c>
       <c r="C16" t="s">
@@ -2788,7 +2799,7 @@
         <v>50</v>
       </c>
       <c r="B17" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR05514152-CC.pdf", "PR05514152-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR05514152-CC.pdf", "PR05514152-CC.pdf")</f>
         <v>PR05514152-CC.pdf</v>
       </c>
       <c r="C17" t="s">
@@ -2809,7 +2820,7 @@
         <v>53</v>
       </c>
       <c r="B18" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR05511832-CC.pdf", "PR05511832-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR05511832-CC.pdf", "PR05511832-CC.pdf")</f>
         <v>PR05511832-CC.pdf</v>
       </c>
       <c r="D18" t="s">
@@ -2827,7 +2838,7 @@
         <v>55</v>
       </c>
       <c r="B19" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR05713422-CC.pdf", "PR05713422-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR05713422-CC.pdf", "PR05713422-CC.pdf")</f>
         <v>PR05713422-CC.pdf</v>
       </c>
       <c r="C19" t="s">
@@ -2848,7 +2859,7 @@
         <v>58</v>
       </c>
       <c r="B20" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR05907184-CC.pdf", "PR05907184-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR05907184-CC.pdf", "PR05907184-CC.pdf")</f>
         <v>PR05907184-CC.pdf</v>
       </c>
       <c r="C20" t="s">
@@ -2869,7 +2880,7 @@
         <v>61</v>
       </c>
       <c r="B21" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR06114350-CC.pdf", "PR06114350-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR06114350-CC.pdf", "PR06114350-CC.pdf")</f>
         <v>PR06114350-CC.pdf</v>
       </c>
       <c r="C21" t="s">
@@ -2890,7 +2901,7 @@
         <v>64</v>
       </c>
       <c r="B22" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR05814617-CC.pdf", "PR05814617-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR05814617-CC.pdf", "PR05814617-CC.pdf")</f>
         <v>PR05814617-CC.pdf</v>
       </c>
       <c r="C22" t="s">
@@ -2911,7 +2922,7 @@
         <v>67</v>
       </c>
       <c r="B23" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR05909642-CC.pdf", "PR05909642-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR05909642-CC.pdf", "PR05909642-CC.pdf")</f>
         <v>PR05909642-CC.pdf</v>
       </c>
       <c r="C23" t="s">
@@ -2932,7 +2943,7 @@
         <v>70</v>
       </c>
       <c r="B24" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR06012475-CC.pdf", "PR06012475-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR06012475-CC.pdf", "PR06012475-CC.pdf")</f>
         <v>PR06012475-CC.pdf</v>
       </c>
       <c r="C24" t="s">
@@ -2953,7 +2964,7 @@
         <v>73</v>
       </c>
       <c r="B25" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR06014617-CC.pdf", "PR06014617-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR06014617-CC.pdf", "PR06014617-CC.pdf")</f>
         <v>PR06014617-CC.pdf</v>
       </c>
       <c r="C25" t="s">
@@ -2974,7 +2985,7 @@
         <v>76</v>
       </c>
       <c r="B26" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR06114956-CC.pdf", "PR06114956-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR06114956-CC.pdf", "PR06114956-CC.pdf")</f>
         <v>PR06114956-CC.pdf</v>
       </c>
       <c r="C26" t="s">
@@ -2995,7 +3006,7 @@
         <v>79</v>
       </c>
       <c r="B27" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR06103808-CC.pdf", "PR06103808-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR06103808-CC.pdf", "PR06103808-CC.pdf")</f>
         <v>PR06103808-CC.pdf</v>
       </c>
       <c r="C27" t="s">
@@ -3016,7 +3027,7 @@
         <v>82</v>
       </c>
       <c r="B28" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-7/PR05009672-CC.pdf", "PR05009672-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-7/PR05009672-CC.pdf", "PR05009672-CC.pdf")</f>
         <v>PR05009672-CC.pdf</v>
       </c>
       <c r="C28" t="s">
@@ -3037,7 +3048,7 @@
         <v>85</v>
       </c>
       <c r="B29" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L090137002-CC.pdf", "L090137002-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L090137002-CC.pdf", "L090137002-CC.pdf")</f>
         <v>L090137002-CC.pdf</v>
       </c>
       <c r="C29" t="s">
@@ -3058,7 +3069,7 @@
         <v>88</v>
       </c>
       <c r="B30" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/SSC1310125-CC.pdf", "SSC1310125-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/SSC1310125-CC.pdf", "SSC1310125-CC.pdf")</f>
         <v>SSC1310125-CC.pdf</v>
       </c>
       <c r="C30" t="s">
@@ -3079,7 +3090,7 @@
         <v>91</v>
       </c>
       <c r="B31" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/Liu_2018_Supercond._Sci._Technol._31_125011-CC.pdf", "Liu_2018_Supercond._Sci._Technol._31_125011-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/Liu_2018_Supercond._Sci._Technol._31_125011-CC.pdf", "Liu_2018_Supercond._Sci._Technol._31_125011-CC.pdf")</f>
         <v>Liu_2018_Supercond._Sci._Technol._31_125011-CC.pdf</v>
       </c>
       <c r="C31" t="s">
@@ -3100,7 +3111,7 @@
         <v>94</v>
       </c>
       <c r="B32" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/EPL0580589.pdf", "EPL0580589.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/EPL0580589.pdf", "EPL0580589.pdf")</f>
         <v>EPL0580589.pdf</v>
       </c>
       <c r="C32" t="s">
@@ -3121,7 +3132,7 @@
         <v>97</v>
       </c>
       <c r="B33" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L088207005-CC.pdf", "L088207005-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L088207005-CC.pdf", "L088207005-CC.pdf")</f>
         <v>L088207005-CC.pdf</v>
       </c>
       <c r="C33" t="s">
@@ -3142,7 +3153,7 @@
         <v>100</v>
       </c>
       <c r="B34" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L089147002-CC.pdf", "L089147002-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L089147002-CC.pdf", "L089147002-CC.pdf")</f>
         <v>L089147002-CC.pdf</v>
       </c>
       <c r="C34" t="s">
@@ -3163,7 +3174,7 @@
         <v>103</v>
       </c>
       <c r="B35" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/APL0774202-CC.pdf", "APL0774202-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/APL0774202-CC.pdf", "APL0774202-CC.pdf")</f>
         <v>APL0774202-CC.pdf</v>
       </c>
       <c r="C35" t="s">
@@ -3184,7 +3195,7 @@
         <v>106</v>
       </c>
       <c r="B36" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/EPL0410207-CC.pdf", "EPL0410207-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/EPL0410207-CC.pdf", "EPL0410207-CC.pdf")</f>
         <v>EPL0410207-CC.pdf</v>
       </c>
       <c r="C36" t="s">
@@ -3205,7 +3216,7 @@
         <v>109</v>
       </c>
       <c r="B37" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/1609.04957-CC.pdf", "1609.04957-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/1609.04957-CC.pdf", "1609.04957-CC.pdf")</f>
         <v>1609.04957-CC.pdf</v>
       </c>
       <c r="C37" t="s">
@@ -3226,7 +3237,7 @@
         <v>112</v>
       </c>
       <c r="B38" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/PhysRevX.9.021044-CC.pdf", "PhysRevX.9.021044-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/PhysRevX.9.021044-CC.pdf", "PhysRevX.9.021044-CC.pdf")</f>
         <v>PhysRevX.9.021044-CC.pdf</v>
       </c>
       <c r="C38" t="s">
@@ -3247,7 +3258,7 @@
         <v>115</v>
       </c>
       <c r="B39" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L093157004-CC.pdf", "L093157004-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L093157004-CC.pdf", "L093157004-CC.pdf")</f>
         <v>L093157004-CC.pdf</v>
       </c>
       <c r="C39" t="s">
@@ -3268,7 +3279,7 @@
         <v>118</v>
       </c>
       <c r="B40" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/SSC1280097-CC.pdf", "SSC1280097-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/SSC1280097-CC.pdf", "SSC1280097-CC.pdf")</f>
         <v>SSC1280097-CC.pdf</v>
       </c>
       <c r="C40" t="s">
@@ -3289,7 +3300,7 @@
         <v>121</v>
       </c>
       <c r="B41" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/JPS081033701-CC.pdf", "JPS081033701-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/JPS081033701-CC.pdf", "JPS081033701-CC.pdf")</f>
         <v>JPS081033701-CC.pdf</v>
       </c>
       <c r="C41" t="s">
@@ -3310,7 +3321,7 @@
         <v>124</v>
       </c>
       <c r="B42" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L088207003-CC.pdf", "L088207003-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L088207003-CC.pdf", "L088207003-CC.pdf")</f>
         <v>L088207003-CC.pdf</v>
       </c>
       <c r="C42" t="s">
@@ -3331,7 +3342,7 @@
         <v>127</v>
       </c>
       <c r="B43" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/SST0180041-CC.pdf", "SST0180041-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/SST0180041-CC.pdf", "SST0180041-CC.pdf")</f>
         <v>SST0180041-CC.pdf</v>
       </c>
       <c r="C43" t="s">
@@ -3352,7 +3363,7 @@
         <v>130</v>
       </c>
       <c r="B44" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L094047006-CC.pdf", "L094047006-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L094047006-CC.pdf", "L094047006-CC.pdf")</f>
         <v>L094047006-CC.pdf</v>
       </c>
       <c r="C44" t="s">
@@ -3373,7 +3384,7 @@
         <v>133</v>
       </c>
       <c r="B45" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L092157004-CC.pdf", "L092157004-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L092157004-CC.pdf", "L092157004-CC.pdf")</f>
         <v>L092157004-CC.pdf</v>
       </c>
       <c r="C45" t="s">
@@ -3394,7 +3405,7 @@
         <v>136</v>
       </c>
       <c r="B46" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/EPJ0290369-CC.pdf", "EPJ0290369-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/EPJ0290369-CC.pdf", "EPJ0290369-CC.pdf")</f>
         <v>EPJ0290369-CC.pdf</v>
       </c>
       <c r="C46" t="s">
@@ -3415,7 +3426,7 @@
         <v>139</v>
       </c>
       <c r="B47" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/SSC1270493-CC.pdf", "SSC1270493-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/SSC1270493-CC.pdf", "SSC1270493-CC.pdf")</f>
         <v>SSC1270493-CC.pdf</v>
       </c>
       <c r="C47" t="s">
@@ -3436,7 +3447,7 @@
         <v>142</v>
       </c>
       <c r="B48" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/SSC1230017-CC.pdf", "SSC1230017-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/SSC1230017-CC.pdf", "SSC1230017-CC.pdf")</f>
         <v>SSC1230017-CC.pdf</v>
       </c>
       <c r="C48" t="s">
@@ -3457,7 +3468,7 @@
         <v>145</v>
       </c>
       <c r="B49" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L094037007-CC.pdf", "L094037007-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L094037007-CC.pdf", "L094037007-CC.pdf")</f>
         <v>L094037007-CC.pdf</v>
       </c>
       <c r="C49" t="s">
@@ -3478,7 +3489,7 @@
         <v>148</v>
       </c>
       <c r="B50" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L088167005-CC.pdf", "L088167005-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L088167005-CC.pdf", "L088167005-CC.pdf")</f>
         <v>L088167005-CC.pdf</v>
       </c>
       <c r="C50" t="s">
@@ -3499,7 +3510,7 @@
         <v>151</v>
       </c>
       <c r="B51" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L095167004-CC.pdf", "L095167004-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L095167004-CC.pdf", "L095167004-CC.pdf")</f>
         <v>L095167004-CC.pdf</v>
       </c>
       <c r="C51" t="s">
@@ -3520,7 +3531,7 @@
         <v>154</v>
       </c>
       <c r="B52" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L091217001-CC.pdf", "L091217001-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L091217001-CC.pdf", "L091217001-CC.pdf")</f>
         <v>L091217001-CC.pdf</v>
       </c>
       <c r="C52" t="s">
@@ -3541,7 +3552,7 @@
         <v>157</v>
       </c>
       <c r="B53" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L092227003-CC.pdf", "L092227003-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L092227003-CC.pdf", "L092227003-CC.pdf")</f>
         <v>L092227003-CC.pdf</v>
       </c>
       <c r="C53" t="s">
@@ -3562,7 +3573,7 @@
         <v>160</v>
       </c>
       <c r="B54" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L094047001-CC.pdf", "L094047001-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L094047001-CC.pdf", "L094047001-CC.pdf")</f>
         <v>L094047001-CC.pdf</v>
       </c>
       <c r="C54" t="s">
@@ -3583,7 +3594,7 @@
         <v>163</v>
       </c>
       <c r="B55" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L088227002-CC.pdf", "L088227002-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L088227002-CC.pdf", "L088227002-CC.pdf")</f>
         <v>L088227002-CC.pdf</v>
       </c>
       <c r="C55" t="s">
@@ -3604,7 +3615,7 @@
         <v>166</v>
       </c>
       <c r="B56" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L090137001-CC.pdf", "L090137001-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L090137001-CC.pdf", "L090137001-CC.pdf")</f>
         <v>L090137001-CC.pdf</v>
       </c>
       <c r="C56" t="s">
@@ -3625,7 +3636,7 @@
         <v>169</v>
       </c>
       <c r="B57" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/JPS081113707-CC.pdf", "JPS081113707-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/JPS081113707-CC.pdf", "JPS081113707-CC.pdf")</f>
         <v>JPS081113707-CC.pdf</v>
       </c>
       <c r="C57" t="s">
@@ -3646,7 +3657,7 @@
         <v>172</v>
       </c>
       <c r="B58" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/Suzuki_etal_2015-CC.pdf", "Suzuki_etal_2015-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/Suzuki_etal_2015-CC.pdf", "Suzuki_etal_2015-CC.pdf")</f>
         <v>Suzuki_etal_2015-CC.pdf</v>
       </c>
       <c r="C58" t="s">
@@ -3667,7 +3678,7 @@
         <v>175</v>
       </c>
       <c r="B59" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/PhysRevX.8.041024-CC.pdf", "PhysRevX.8.041024-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/PhysRevX.8.041024-CC.pdf", "PhysRevX.8.041024-CC.pdf")</f>
         <v>PhysRevX.8.041024-CC.pdf</v>
       </c>
       <c r="C59" t="s">
@@ -3688,7 +3699,7 @@
         <v>178</v>
       </c>
       <c r="B60" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/EPL0330153-CC.pdf", "EPL0330153-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/EPL0330153-CC.pdf", "EPL0330153-CC.pdf")</f>
         <v>EPL0330153-CC.pdf</v>
       </c>
       <c r="C60" t="s">
@@ -3709,7 +3720,7 @@
         <v>181</v>
       </c>
       <c r="B61" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L089157004-CC.pdf", "L089157004-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L089157004-CC.pdf", "L089157004-CC.pdf")</f>
         <v>L089157004-CC.pdf</v>
       </c>
       <c r="C61" t="s">
@@ -3730,7 +3741,7 @@
         <v>184</v>
       </c>
       <c r="B62" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L095117006-CC.pdf", "L095117006-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L095117006-CC.pdf", "L095117006-CC.pdf")</f>
         <v>L095117006-CC.pdf</v>
       </c>
       <c r="C62" t="s">
@@ -3751,7 +3762,7 @@
         <v>187</v>
       </c>
       <c r="B63" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/Carnicom_2018_Supercond._Sci._Technol._31_115005.pdf", "Carnicom_2018_Supercond._Sci._Technol._31_115005.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/Carnicom_2018_Supercond._Sci._Technol._31_115005.pdf", "Carnicom_2018_Supercond._Sci._Technol._31_115005.pdf")</f>
         <v>Carnicom_2018_Supercond._Sci._Technol._31_115005.pdf</v>
       </c>
       <c r="C63" t="s">
@@ -3772,7 +3783,7 @@
         <v>190</v>
       </c>
       <c r="B64" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/Li_2018_Supercond._Sci._Technol._31_085001.pdf", "Li_2018_Supercond._Sci._Technol._31_085001.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/Li_2018_Supercond._Sci._Technol._31_085001.pdf", "Li_2018_Supercond._Sci._Technol._31_085001.pdf")</f>
         <v>Li_2018_Supercond._Sci._Technol._31_085001.pdf</v>
       </c>
       <c r="C64" t="s">
@@ -3793,7 +3804,7 @@
         <v>193</v>
       </c>
       <c r="B65" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L094127001-CC.pdf", "L094127001-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L094127001-CC.pdf", "L094127001-CC.pdf")</f>
         <v>L094127001-CC.pdf</v>
       </c>
       <c r="C65" t="s">
@@ -3814,7 +3825,7 @@
         <v>196</v>
       </c>
       <c r="B66" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L091087001-CC.pdf", "L091087001-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L091087001-CC.pdf", "L091087001-CC.pdf")</f>
         <v>L091087001-CC.pdf</v>
       </c>
       <c r="C66" t="s">
@@ -3835,7 +3846,7 @@
         <v>199</v>
       </c>
       <c r="B67" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/Tanaka_etal_2017-CC.pdf", "Tanaka_etal_2017-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/Tanaka_etal_2017-CC.pdf", "Tanaka_etal_2017-CC.pdf")</f>
         <v>Tanaka_etal_2017-CC.pdf</v>
       </c>
       <c r="C67" t="s">
@@ -3856,7 +3867,7 @@
         <v>202</v>
       </c>
       <c r="B68" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/L093156802-CC.pdf", "L093156802-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/L093156802-CC.pdf", "L093156802-CC.pdf")</f>
         <v>L093156802-CC.pdf</v>
       </c>
       <c r="C68" t="s">
@@ -3877,7 +3888,7 @@
         <v>205</v>
       </c>
       <c r="B69" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/Drozdov_etal_2015.pdf", "Drozdov_etal_2015.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/Drozdov_etal_2015.pdf", "Drozdov_etal_2015.pdf")</f>
         <v>Drozdov_etal_2015.pdf</v>
       </c>
       <c r="C69" t="s">
@@ -3895,7 +3906,7 @@
         <v>207</v>
       </c>
       <c r="B70" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/1903.04321-CC.pdf", "1903.04321-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/1903.04321-CC.pdf", "1903.04321-CC.pdf")</f>
         <v>1903.04321-CC.pdf</v>
       </c>
       <c r="C70" t="s">
@@ -3916,7 +3927,7 @@
         <v>210</v>
       </c>
       <c r="B71" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-1/SST01600L7-CC.pdf", "SST01600L7-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-1/SST01600L7-CC.pdf", "SST01600L7-CC.pdf")</f>
         <v>SST01600L7-CC.pdf</v>
       </c>
       <c r="C71" t="s">
@@ -3937,7 +3948,7 @@
         <v>213</v>
       </c>
       <c r="B72" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-6/sun2012re-emerging-CC.pdf", "sun2012re-emerging-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-6/sun2012re-emerging-CC.pdf", "sun2012re-emerging-CC.pdf")</f>
         <v>sun2012re-emerging-CC.pdf</v>
       </c>
       <c r="C72" t="s">
@@ -3958,7 +3969,7 @@
         <v>216</v>
       </c>
       <c r="B73" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-6/xing2014theAnomaly-CC.pdf", "xing2014theAnomaly-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-6/xing2014theAnomaly-CC.pdf", "xing2014theAnomaly-CC.pdf")</f>
         <v>xing2014theAnomaly-CC.pdf</v>
       </c>
       <c r="C73" t="s">
@@ -3979,7 +3990,7 @@
         <v>219</v>
       </c>
       <c r="B74" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-6/yamaguchi2014ac.pdf", "yamaguchi2014ac.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-6/yamaguchi2014ac.pdf", "yamaguchi2014ac.pdf")</f>
         <v>yamaguchi2014ac.pdf</v>
       </c>
       <c r="C74" t="s">
@@ -4000,7 +4011,7 @@
         <v>222</v>
       </c>
       <c r="B75" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-6/kotegawa2008abrupt-CC.pdf", "kotegawa2008abrupt-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-6/kotegawa2008abrupt-CC.pdf", "kotegawa2008abrupt-CC.pdf")</f>
         <v>kotegawa2008abrupt-CC.pdf</v>
       </c>
       <c r="C75" t="s">
@@ -4021,7 +4032,7 @@
         <v>225</v>
       </c>
       <c r="B76" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-6/mydeen2010temperature-CC.pdf", "mydeen2010temperature-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-6/mydeen2010temperature-CC.pdf", "mydeen2010temperature-CC.pdf")</f>
         <v>mydeen2010temperature-CC.pdf</v>
       </c>
       <c r="C76" t="s">
@@ -4039,7 +4050,7 @@
         <v>227</v>
       </c>
       <c r="B77" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-6/piva2015combined-CC.pdf", "piva2015combined-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-6/piva2015combined-CC.pdf", "piva2015combined-CC.pdf")</f>
         <v>piva2015combined-CC.pdf</v>
       </c>
       <c r="C77" t="s">
@@ -4060,7 +4071,7 @@
         <v>230</v>
       </c>
       <c r="B78" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-6/wang2011effect.pdf", "wang2011effect.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-6/wang2011effect.pdf", "wang2011effect.pdf")</f>
         <v>wang2011effect.pdf</v>
       </c>
       <c r="C78" t="s">
@@ -4081,7 +4092,7 @@
         <v>233</v>
       </c>
       <c r="B79" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-6/ivanovskii2008newHigh.pdf", "ivanovskii2008newHigh.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-6/ivanovskii2008newHigh.pdf", "ivanovskii2008newHigh.pdf")</f>
         <v>ivanovskii2008newHigh.pdf</v>
       </c>
       <c r="C79" t="s">
@@ -4102,7 +4113,7 @@
         <v>236</v>
       </c>
       <c r="B80" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-6/ying2011pressure-CC.pdf", "ying2011pressure-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-6/ying2011pressure-CC.pdf", "ying2011pressure-CC.pdf")</f>
         <v>ying2011pressure-CC.pdf</v>
       </c>
       <c r="C80" t="s">
@@ -4123,7 +4134,7 @@
         <v>239</v>
       </c>
       <c r="B81" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-6/chu2009high-CC.pdf", "chu2009high-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-6/chu2009high-CC.pdf", "chu2009high-CC.pdf")</f>
         <v>chu2009high-CC.pdf</v>
       </c>
       <c r="C81" t="s">
@@ -4144,7 +4155,7 @@
         <v>242</v>
       </c>
       <c r="B82" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-6/okada2008supercondctivity-CC.pdf", "okada2008supercondctivity-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-6/okada2008supercondctivity-CC.pdf", "okada2008supercondctivity-CC.pdf")</f>
         <v>okada2008supercondctivity-CC.pdf</v>
       </c>
       <c r="C82" t="s">
@@ -4165,7 +4176,7 @@
         <v>245</v>
       </c>
       <c r="B83" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-6/hott2013review-CC.pdf", "hott2013review-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-6/hott2013review-CC.pdf", "hott2013review-CC.pdf")</f>
         <v>hott2013review-CC.pdf</v>
       </c>
       <c r="C83" t="s">
@@ -4183,7 +4194,7 @@
         <v>247</v>
       </c>
       <c r="B84" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-6/kotegawa2009contrasting-CC.pdf", "kotegawa2009contrasting-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-6/kotegawa2009contrasting-CC.pdf", "kotegawa2009contrasting-CC.pdf")</f>
         <v>kotegawa2009contrasting-CC.pdf</v>
       </c>
       <c r="C84" t="s">
@@ -4204,7 +4215,7 @@
         <v>250</v>
       </c>
       <c r="B85" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-8/1802.09882-CC.pdf", "1802.09882-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-8/1802.09882-CC.pdf", "1802.09882-CC.pdf")</f>
         <v>1802.09882-CC.pdf</v>
       </c>
       <c r="C85" t="s">
@@ -4225,7 +4236,7 @@
         <v>253</v>
       </c>
       <c r="B86" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-8/HfV2O431805.08285-CC.pdf", "HfV2O431805.08285-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-8/HfV2O431805.08285-CC.pdf", "HfV2O431805.08285-CC.pdf")</f>
         <v>HfV2O431805.08285-CC.pdf</v>
       </c>
       <c r="C86" t="s">
@@ -4246,7 +4257,7 @@
         <v>256</v>
       </c>
       <c r="B87" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-8/Rb2Cr3As3_quasi1D_SC1412.2596-CC.pdf", "Rb2Cr3As3_quasi1D_SC1412.2596-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-8/Rb2Cr3As3_quasi1D_SC1412.2596-CC.pdf", "Rb2Cr3As3_quasi1D_SC1412.2596-CC.pdf")</f>
         <v>Rb2Cr3As3_quasi1D_SC1412.2596-CC.pdf</v>
       </c>
       <c r="C87" t="s">
@@ -4267,7 +4278,7 @@
         <v>259</v>
       </c>
       <c r="B88" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-8/SCinTiO_1612.02502-CC.pdf", "SCinTiO_1612.02502-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-8/SCinTiO_1612.02502-CC.pdf", "SCinTiO_1612.02502-CC.pdf")</f>
         <v>SCinTiO_1612.02502-CC.pdf</v>
       </c>
       <c r="C88" t="s">
@@ -4288,7 +4299,7 @@
         <v>262</v>
       </c>
       <c r="B89" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-8/CoA4_HTSC_theory1807.00934-CC.pdf", "CoA4_HTSC_theory1807.00934-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-8/CoA4_HTSC_theory1807.00934-CC.pdf", "CoA4_HTSC_theory1807.00934-CC.pdf")</f>
         <v>CoA4_HTSC_theory1807.00934-CC.pdf</v>
       </c>
       <c r="C89" t="s">
@@ -4309,7 +4320,7 @@
         <v>265</v>
       </c>
       <c r="B90" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-8/1802.03907-CC.pdf", "1802.03907-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-8/1802.03907-CC.pdf", "1802.03907-CC.pdf")</f>
         <v>1802.03907-CC.pdf</v>
       </c>
       <c r="C90" t="s">
@@ -4330,7 +4341,7 @@
         <v>268</v>
       </c>
       <c r="B91" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-8/Tc4k_interfaceBi_Ni-CC.pdf", "Tc4k_interfaceBi_Ni-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-8/Tc4k_interfaceBi_Ni-CC.pdf", "Tc4k_interfaceBi_Ni-CC.pdf")</f>
         <v>Tc4k_interfaceBi_Ni-CC.pdf</v>
       </c>
       <c r="C91" t="s">
@@ -4351,7 +4362,7 @@
         <v>271</v>
       </c>
       <c r="B92" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/MAT0305503-CC.pdf", "MAT0305503-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/MAT0305503-CC.pdf", "MAT0305503-CC.pdf")</f>
         <v>MAT0305503-CC.pdf</v>
       </c>
       <c r="C92" t="s">
@@ -4372,7 +4383,7 @@
         <v>274</v>
       </c>
       <c r="B93" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/P066214509-CC.pdf", "P066214509-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/P066214509-CC.pdf", "P066214509-CC.pdf")</f>
         <v>P066214509-CC.pdf</v>
       </c>
       <c r="C93" t="s">
@@ -4393,7 +4404,7 @@
         <v>277</v>
       </c>
       <c r="B94" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/P066104528-CC.pdf", "P066104528-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/P066104528-CC.pdf", "P066104528-CC.pdf")</f>
         <v>P066104528-CC.pdf</v>
       </c>
       <c r="C94" t="s">
@@ -4414,7 +4425,7 @@
         <v>280</v>
       </c>
       <c r="B95" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/P065104523-CC.pdf", "P065104523-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/P065104523-CC.pdf", "P065104523-CC.pdf")</f>
         <v>P065104523-CC.pdf</v>
       </c>
       <c r="C95" t="s">
@@ -4435,7 +4446,7 @@
         <v>283</v>
       </c>
       <c r="B96" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/P065172501-CC.pdf", "P065172501-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/P065172501-CC.pdf", "P065172501-CC.pdf")</f>
         <v>P065172501-CC.pdf</v>
       </c>
       <c r="C96" t="s">
@@ -4456,7 +4467,7 @@
         <v>286</v>
       </c>
       <c r="B97" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/P064144524-CC.pdf", "P064144524-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/P064144524-CC.pdf", "P064144524-CC.pdf")</f>
         <v>P064144524-CC.pdf</v>
       </c>
       <c r="C97" t="s">
@@ -4477,7 +4488,7 @@
         <v>289</v>
       </c>
       <c r="B98" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/MAT0106521-CC.pdf", "MAT0106521-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/MAT0106521-CC.pdf", "MAT0106521-CC.pdf")</f>
         <v>MAT0106521-CC.pdf</v>
       </c>
       <c r="C98" t="s">
@@ -4498,7 +4509,7 @@
         <v>292</v>
       </c>
       <c r="B99" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/MCP0750110-CC.pdf", "MCP0750110-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/MCP0750110-CC.pdf", "MCP0750110-CC.pdf")</f>
         <v>MCP0750110-CC.pdf</v>
       </c>
       <c r="C99" t="s">
@@ -4519,7 +4530,7 @@
         <v>295</v>
       </c>
       <c r="B100" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/P066024503-CC.pdf", "P066024503-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/P066024503-CC.pdf", "P066024503-CC.pdf")</f>
         <v>P066024503-CC.pdf</v>
       </c>
       <c r="C100" t="s">
@@ -4540,7 +4551,7 @@
         <v>298</v>
       </c>
       <c r="B101" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/MPL0150497-CC.pdf", "MPL0150497-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/MPL0150497-CC.pdf", "MPL0150497-CC.pdf")</f>
         <v>MPL0150497-CC.pdf</v>
       </c>
       <c r="C101" t="s">
@@ -4561,7 +4572,7 @@
         <v>301</v>
       </c>
       <c r="B102" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/NAT3500600.pdf", "NAT3500600.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/NAT3500600.pdf", "NAT3500600.pdf")</f>
         <v>NAT3500600.pdf</v>
       </c>
       <c r="C102" t="s">
@@ -4582,7 +4593,7 @@
         <v>304</v>
       </c>
       <c r="B103" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/P067104503-CC.pdf", "P067104503-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/P067104503-CC.pdf", "P067104503-CC.pdf")</f>
         <v>P067104503-CC.pdf</v>
       </c>
       <c r="C103" t="s">
@@ -4603,7 +4614,7 @@
         <v>307</v>
       </c>
       <c r="B104" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/P063224522-CC.pdf", "P063224522-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/P063224522-CC.pdf", "P063224522-CC.pdf")</f>
         <v>P063224522-CC.pdf</v>
       </c>
       <c r="C104" t="s">
@@ -4624,7 +4635,7 @@
         <v>310</v>
       </c>
       <c r="B105" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/P065224520-CC.pdf", "P065224520-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/P065224520-CC.pdf", "P065224520-CC.pdf")</f>
         <v>P065224520-CC.pdf</v>
       </c>
       <c r="C105" t="s">
@@ -4645,7 +4656,7 @@
         <v>313</v>
       </c>
       <c r="B106" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/P064172514-CC.pdf", "P064172514-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/P064172514-CC.pdf", "P064172514-CC.pdf")</f>
         <v>P064172514-CC.pdf</v>
       </c>
       <c r="C106" t="s">
@@ -4666,7 +4677,7 @@
         <v>316</v>
       </c>
       <c r="B107" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/P067172501-CC.pdf", "P067172501-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/P067172501-CC.pdf", "P067172501-CC.pdf")</f>
         <v>P067172501-CC.pdf</v>
       </c>
       <c r="C107" t="s">
@@ -4687,7 +4698,7 @@
         <v>319</v>
       </c>
       <c r="B108" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/P066020503-CC.pdf", "P066020503-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/P066020503-CC.pdf", "P066020503-CC.pdf")</f>
         <v>P066020503-CC.pdf</v>
       </c>
       <c r="C108" t="s">
@@ -4708,7 +4719,7 @@
         <v>322</v>
       </c>
       <c r="B109" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/P066132510-CC.pdf", "P066132510-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/P066132510-CC.pdf", "P066132510-CC.pdf")</f>
         <v>P066132510-CC.pdf</v>
       </c>
       <c r="C109" t="s">
@@ -4729,7 +4740,7 @@
         <v>325</v>
       </c>
       <c r="B110" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/P065024523-CC.pdf", "P065024523-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/P065024523-CC.pdf", "P065024523-CC.pdf")</f>
         <v>P065024523-CC.pdf</v>
       </c>
       <c r="C110" t="s">
@@ -4747,7 +4758,7 @@
         <v>327</v>
       </c>
       <c r="B111" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/P066020501-CC.pdf", "P066020501-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/P066020501-CC.pdf", "P066020501-CC.pdf")</f>
         <v>P066020501-CC.pdf</v>
       </c>
       <c r="C111" t="s">
@@ -4768,7 +4779,7 @@
         <v>330</v>
       </c>
       <c r="B112" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-3/P066024502-CC.pdf", "P066024502-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-3/P066024502-CC.pdf", "P066024502-CC.pdf")</f>
         <v>P066024502-CC.pdf</v>
       </c>
       <c r="C112" t="s">
@@ -4789,7 +4800,7 @@
         <v>333</v>
       </c>
       <c r="B113" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P070184523-CC.pdf", "P070184523-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P070184523-CC.pdf", "P070184523-CC.pdf")</f>
         <v>P070184523-CC.pdf</v>
       </c>
       <c r="C113" t="s">
@@ -4810,7 +4821,7 @@
         <v>336</v>
       </c>
       <c r="B114" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P072064520-CC.pdf", "P072064520-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P072064520-CC.pdf", "P072064520-CC.pdf")</f>
         <v>P072064520-CC.pdf</v>
       </c>
       <c r="C114" t="s">
@@ -4831,7 +4842,7 @@
         <v>339</v>
       </c>
       <c r="B115" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P068100502-CC.pdf", "P068100502-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P068100502-CC.pdf", "P068100502-CC.pdf")</f>
         <v>P068100502-CC.pdf</v>
       </c>
       <c r="C115" t="s">
@@ -4849,7 +4860,7 @@
         <v>341</v>
       </c>
       <c r="B116" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P069184513-CC.pdf", "P069184513-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P069184513-CC.pdf", "P069184513-CC.pdf")</f>
         <v>P069184513-CC.pdf</v>
       </c>
       <c r="C116" t="s">
@@ -4870,7 +4881,7 @@
         <v>344</v>
       </c>
       <c r="B117" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P071134526-CC.pdf", "P071134526-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P071134526-CC.pdf", "P071134526-CC.pdf")</f>
         <v>P071134526-CC.pdf</v>
       </c>
       <c r="C117" t="s">
@@ -4891,7 +4902,7 @@
         <v>347</v>
       </c>
       <c r="B118" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P070020503-CC.pdf", "P070020503-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P070020503-CC.pdf", "P070020503-CC.pdf")</f>
         <v>P070020503-CC.pdf</v>
       </c>
       <c r="C118" t="s">
@@ -4912,7 +4923,7 @@
         <v>350</v>
       </c>
       <c r="B119" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P072174508-CC.pdf", "P072174508-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P072174508-CC.pdf", "P072174508-CC.pdf")</f>
         <v>P072174508-CC.pdf</v>
       </c>
       <c r="C119" t="s">
@@ -4933,7 +4944,7 @@
         <v>353</v>
       </c>
       <c r="B120" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P072214523-CC.pdf", "P072214523-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P072214523-CC.pdf", "P072214523-CC.pdf")</f>
         <v>P072214523-CC.pdf</v>
       </c>
       <c r="C120" t="s">
@@ -4954,7 +4965,7 @@
         <v>356</v>
       </c>
       <c r="B121" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/PHC1910237.pdf", "PHC1910237.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/PHC1910237.pdf", "PHC1910237.pdf")</f>
         <v>PHC1910237.pdf</v>
       </c>
       <c r="C121" t="s">
@@ -4975,7 +4986,7 @@
         <v>359</v>
       </c>
       <c r="B122" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P068132504-CC.pdf", "P068132504-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P068132504-CC.pdf", "P068132504-CC.pdf")</f>
         <v>P068132504-CC.pdf</v>
       </c>
       <c r="C122" t="s">
@@ -4996,7 +5007,7 @@
         <v>362</v>
       </c>
       <c r="B123" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P068064507-CC.pdf", "P068064507-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P068064507-CC.pdf", "P068064507-CC.pdf")</f>
         <v>P068064507-CC.pdf</v>
       </c>
       <c r="C123" t="s">
@@ -5017,7 +5028,7 @@
         <v>365</v>
       </c>
       <c r="B124" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P071100502-CC.pdf", "P071100502-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P071100502-CC.pdf", "P071100502-CC.pdf")</f>
         <v>P071100502-CC.pdf</v>
       </c>
       <c r="C124" t="s">
@@ -5038,7 +5049,7 @@
         <v>368</v>
       </c>
       <c r="B125" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P072094504-CC.pdf", "P072094504-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P072094504-CC.pdf", "P072094504-CC.pdf")</f>
         <v>P072094504-CC.pdf</v>
       </c>
       <c r="C125" t="s">
@@ -5056,7 +5067,7 @@
         <v>370</v>
       </c>
       <c r="B126" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P071104513-CC.pdf", "P071104513-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P071104513-CC.pdf", "P071104513-CC.pdf")</f>
         <v>P071104513-CC.pdf</v>
       </c>
       <c r="C126" t="s">
@@ -5077,7 +5088,7 @@
         <v>373</v>
       </c>
       <c r="B127" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P072104504-CC.pdf", "P072104504-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P072104504-CC.pdf", "P072104504-CC.pdf")</f>
         <v>P072104504-CC.pdf</v>
       </c>
       <c r="C127" t="s">
@@ -5098,7 +5109,7 @@
         <v>376</v>
       </c>
       <c r="B128" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P069014507-CC.pdf", "P069014507-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P069014507-CC.pdf", "P069014507-CC.pdf")</f>
         <v>P069014507-CC.pdf</v>
       </c>
       <c r="D128" t="s">
@@ -5116,7 +5127,7 @@
         <v>378</v>
       </c>
       <c r="B129" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P072220505-CC.pdf", "P072220505-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P072220505-CC.pdf", "P072220505-CC.pdf")</f>
         <v>P072220505-CC.pdf</v>
       </c>
       <c r="C129" t="s">
@@ -5137,7 +5148,7 @@
         <v>381</v>
       </c>
       <c r="B130" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P070052502-CC.pdf", "P070052502-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P070052502-CC.pdf", "P070052502-CC.pdf")</f>
         <v>P070052502-CC.pdf</v>
       </c>
       <c r="D130" t="s">
@@ -5155,7 +5166,7 @@
         <v>383</v>
       </c>
       <c r="B131" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/PHC1580178.pdf", "PHC1580178.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/PHC1580178.pdf", "PHC1580178.pdf")</f>
         <v>PHC1580178.pdf</v>
       </c>
       <c r="C131" t="s">
@@ -5176,7 +5187,7 @@
         <v>386</v>
       </c>
       <c r="B132" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P072014504-CC.pdf", "P072014504-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P072014504-CC.pdf", "P072014504-CC.pdf")</f>
         <v>P072014504-CC.pdf</v>
       </c>
       <c r="C132" t="s">
@@ -5197,7 +5208,7 @@
         <v>389</v>
       </c>
       <c r="B133" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/PHC1580183-CC.pdf", "PHC1580183-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/PHC1580183-CC.pdf", "PHC1580183-CC.pdf")</f>
         <v>PHC1580183-CC.pdf</v>
       </c>
       <c r="C133" t="s">
@@ -5218,7 +5229,7 @@
         <v>392</v>
       </c>
       <c r="B134" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/PHB1480442.pdf", "PHB1480442.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/PHB1480442.pdf", "PHB1480442.pdf")</f>
         <v>PHB1480442.pdf</v>
       </c>
       <c r="C134" t="s">
@@ -5239,7 +5250,7 @@
         <v>395</v>
       </c>
       <c r="B135" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P069174506-CC.pdf", "P069174506-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P069174506-CC.pdf", "P069174506-CC.pdf")</f>
         <v>P069174506-CC.pdf</v>
       </c>
       <c r="C135" t="s">
@@ -5260,7 +5271,7 @@
         <v>398</v>
       </c>
       <c r="B136" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P068132507-CC.pdf", "P068132507-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P068132507-CC.pdf", "P068132507-CC.pdf")</f>
         <v>P068132507-CC.pdf</v>
       </c>
       <c r="C136" t="s">
@@ -5281,7 +5292,7 @@
         <v>401</v>
       </c>
       <c r="B137" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P070054519-CC.pdf", "P070054519-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P070054519-CC.pdf", "P070054519-CC.pdf")</f>
         <v>P070054519-CC.pdf</v>
       </c>
       <c r="C137" t="s">
@@ -5302,7 +5313,7 @@
         <v>404</v>
       </c>
       <c r="B138" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P071104516-CC.pdf", "P071104516-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P071104516-CC.pdf", "P071104516-CC.pdf")</f>
         <v>P071104516-CC.pdf</v>
       </c>
       <c r="C138" t="s">
@@ -5320,7 +5331,7 @@
         <v>406</v>
       </c>
       <c r="B139" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P068214517-CC.pdf", "P068214517-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P068214517-CC.pdf", "P068214517-CC.pdf")</f>
         <v>P068214517-CC.pdf</v>
       </c>
       <c r="C139" t="s">
@@ -5341,7 +5352,7 @@
         <v>409</v>
       </c>
       <c r="B140" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/PHC1480411-CC.pdf", "PHC1480411-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/PHC1480411-CC.pdf", "PHC1480411-CC.pdf")</f>
         <v>PHC1480411-CC.pdf</v>
       </c>
       <c r="C140" t="s">
@@ -5362,7 +5373,7 @@
         <v>412</v>
       </c>
       <c r="B141" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P070214505-CC.pdf", "P070214505-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P070214505-CC.pdf", "P070214505-CC.pdf")</f>
         <v>P070214505-CC.pdf</v>
       </c>
       <c r="C141" t="s">
@@ -5380,7 +5391,7 @@
         <v>414</v>
       </c>
       <c r="B142" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P072224509-CC.pdf", "P072224509-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P072224509-CC.pdf", "P072224509-CC.pdf")</f>
         <v>P072224509-CC.pdf</v>
       </c>
       <c r="C142" t="s">
@@ -5401,7 +5412,7 @@
         <v>417</v>
       </c>
       <c r="B143" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P072064527-CC.pdf", "P072064527-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P072064527-CC.pdf", "P072064527-CC.pdf")</f>
         <v>P072064527-CC.pdf</v>
       </c>
       <c r="C143" t="s">
@@ -5422,7 +5433,7 @@
         <v>420</v>
       </c>
       <c r="B144" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/PCS2739-CC.pdf", "PCS2739-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/PCS2739-CC.pdf", "PCS2739-CC.pdf")</f>
         <v>PCS2739-CC.pdf</v>
       </c>
       <c r="C144" t="s">
@@ -5443,7 +5454,7 @@
         <v>423</v>
       </c>
       <c r="B145" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P071184510-CC.pdf", "P071184510-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P071184510-CC.pdf", "P071184510-CC.pdf")</f>
         <v>P071184510-CC.pdf</v>
       </c>
       <c r="C145" t="s">
@@ -5464,7 +5475,7 @@
         <v>426</v>
       </c>
       <c r="B146" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P072180504-CC.pdf", "P072180504-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P072180504-CC.pdf", "P072180504-CC.pdf")</f>
         <v>P072180504-CC.pdf</v>
       </c>
       <c r="C146" t="s">
@@ -5485,7 +5496,7 @@
         <v>429</v>
       </c>
       <c r="B147" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-4/P068180505-CC.pdf", "P068180505-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-4/P068180505-CC.pdf", "P068180505-CC.pdf")</f>
         <v>P068180505-CC.pdf</v>
       </c>
       <c r="C147" t="s">
@@ -5506,7 +5517,7 @@
         <v>432</v>
       </c>
       <c r="B148" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC4210001-CC.pdf", "PHC4210001-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC4210001-CC.pdf", "PHC4210001-CC.pdf")</f>
         <v>PHC4210001-CC.pdf</v>
       </c>
       <c r="C148" t="s">
@@ -5527,7 +5538,7 @@
         <v>435</v>
       </c>
       <c r="B149" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC1980027.pdf", "PHC1980027.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC1980027.pdf", "PHC1980027.pdf")</f>
         <v>PHC1980027.pdf</v>
       </c>
       <c r="C149" t="s">
@@ -5548,7 +5559,7 @@
         <v>438</v>
       </c>
       <c r="B150" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC4020027-CC.pdf", "PHC4020027-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC4020027-CC.pdf", "PHC4020027-CC.pdf")</f>
         <v>PHC4020027-CC.pdf</v>
       </c>
       <c r="C150" t="s">
@@ -5569,7 +5580,7 @@
         <v>441</v>
       </c>
       <c r="B151" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC3410729-CC.pdf", "PHC3410729-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC3410729-CC.pdf", "PHC3410729-CC.pdf")</f>
         <v>PHC3410729-CC.pdf</v>
       </c>
       <c r="C151" t="s">
@@ -5590,7 +5601,7 @@
         <v>444</v>
       </c>
       <c r="B152" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC3660299-CC.pdf", "PHC3660299-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC3660299-CC.pdf", "PHC3660299-CC.pdf")</f>
         <v>PHC3660299-CC.pdf</v>
       </c>
       <c r="C152" t="s">
@@ -5611,7 +5622,7 @@
         <v>447</v>
       </c>
       <c r="B153" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC3130001-CC.pdf", "PHC3130001-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC3130001-CC.pdf", "PHC3130001-CC.pdf")</f>
         <v>PHC3130001-CC.pdf</v>
       </c>
       <c r="C153" t="s">
@@ -5632,7 +5643,7 @@
         <v>450</v>
       </c>
       <c r="B154" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC2640145-CC.pdf", "PHC2640145-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC2640145-CC.pdf", "PHC2640145-CC.pdf")</f>
         <v>PHC2640145-CC.pdf</v>
       </c>
       <c r="C154" t="s">
@@ -5653,7 +5664,7 @@
         <v>453</v>
       </c>
       <c r="B155" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC2240263-CC.pdf", "PHC2240263-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC2240263-CC.pdf", "PHC2240263-CC.pdf")</f>
         <v>PHC2240263-CC.pdf</v>
       </c>
       <c r="C155" t="s">
@@ -5674,7 +5685,7 @@
         <v>456</v>
       </c>
       <c r="B156" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC3910237-CC.pdf", "PHC3910237-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC3910237-CC.pdf", "PHC3910237-CC.pdf")</f>
         <v>PHC3910237-CC.pdf</v>
       </c>
       <c r="C156" t="s">
@@ -5695,7 +5706,7 @@
         <v>459</v>
       </c>
       <c r="B157" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC4020152-CC.pdf", "PHC4020152-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC4020152-CC.pdf", "PHC4020152-CC.pdf")</f>
         <v>PHC4020152-CC.pdf</v>
       </c>
       <c r="C157" t="s">
@@ -5716,7 +5727,7 @@
         <v>462</v>
       </c>
       <c r="B158" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC4320193-CC.pdf", "PHC4320193-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC4320193-CC.pdf", "PHC4320193-CC.pdf")</f>
         <v>PHC4320193-CC.pdf</v>
       </c>
       <c r="C158" t="s">
@@ -5737,7 +5748,7 @@
         <v>465</v>
       </c>
       <c r="B159" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC3830337-CC.pdf", "PHC3830337-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC3830337-CC.pdf", "PHC3830337-CC.pdf")</f>
         <v>PHC3830337-CC.pdf</v>
       </c>
       <c r="C159" t="s">
@@ -5758,7 +5769,7 @@
         <v>468</v>
       </c>
       <c r="B160" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC4030200-CC.pdf", "PHC4030200-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC4030200-CC.pdf", "PHC4030200-CC.pdf")</f>
         <v>PHC4030200-CC.pdf</v>
       </c>
       <c r="C160" t="s">
@@ -5779,7 +5790,7 @@
         <v>471</v>
       </c>
       <c r="B161" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC3200009-CC.pdf", "PHC3200009-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC3200009-CC.pdf", "PHC3200009-CC.pdf")</f>
         <v>PHC3200009-CC.pdf</v>
       </c>
       <c r="C161" t="s">
@@ -5800,7 +5811,7 @@
         <v>474</v>
       </c>
       <c r="B162" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC4170033-CC.pdf", "PHC4170033-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC4170033-CC.pdf", "PHC4170033-CC.pdf")</f>
         <v>PHC4170033-CC.pdf</v>
       </c>
       <c r="C162" t="s">
@@ -5821,7 +5832,7 @@
         <v>477</v>
       </c>
       <c r="B163" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC3411655-CC.pdf", "PHC3411655-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC3411655-CC.pdf", "PHC3411655-CC.pdf")</f>
         <v>PHC3411655-CC.pdf</v>
       </c>
       <c r="C163" t="s">
@@ -5842,7 +5853,7 @@
         <v>480</v>
       </c>
       <c r="B164" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-5/PHC4200023-CC.pdf", "PHC4200023-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-5/PHC4200023-CC.pdf", "PHC4200023-CC.pdf")</f>
         <v>PHC4200023-CC.pdf</v>
       </c>
       <c r="C164" t="s">
@@ -5863,7 +5874,7 @@
         <v>483</v>
       </c>
       <c r="B165" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-2/JP01103169-CC.pdf", "JP01103169-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-2/JP01103169-CC.pdf", "JP01103169-CC.pdf")</f>
         <v>JP01103169-CC.pdf</v>
       </c>
       <c r="C165" t="s">
@@ -5884,7 +5895,7 @@
         <v>486</v>
       </c>
       <c r="B166" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-2/JPS0730819-CC.pdf", "JPS0730819-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-2/JPS0730819-CC.pdf", "JPS0730819-CC.pdf")</f>
         <v>JPS0730819-CC.pdf</v>
       </c>
       <c r="C166" t="s">
@@ -5905,7 +5916,7 @@
         <v>489</v>
       </c>
       <c r="B167" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-2/JPS0731655-CC.pdf", "JPS0731655-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-2/JPS0731655-CC.pdf", "JPS0731655-CC.pdf")</f>
         <v>JPS0731655-CC.pdf</v>
       </c>
       <c r="C167" t="s">
@@ -5926,7 +5937,7 @@
         <v>492</v>
       </c>
       <c r="B168" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-2/JPS0732912-CC.pdf", "JPS0732912-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-2/JPS0732912-CC.pdf", "JPS0732912-CC.pdf")</f>
         <v>JPS0732912-CC.pdf</v>
       </c>
       <c r="C168" t="s">
@@ -5944,7 +5955,7 @@
         <v>494</v>
       </c>
       <c r="B169" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-2/JPS0731297-CC.pdf", "JPS0731297-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-2/JPS0731297-CC.pdf", "JPS0731297-CC.pdf")</f>
         <v>JPS0731297-CC.pdf</v>
       </c>
       <c r="C169" t="s">
@@ -5965,7 +5976,7 @@
         <v>497</v>
       </c>
       <c r="B170" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-2/JPS0723041-CC.pdf", "JPS0723041-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-2/JPS0723041-CC.pdf", "JPS0723041-CC.pdf")</f>
         <v>JPS0723041-CC.pdf</v>
       </c>
       <c r="C170" t="s">
@@ -5986,7 +5997,7 @@
         <v>500</v>
       </c>
       <c r="B171" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-2/JPC0150L17-CC.pdf", "JPC0150L17-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-2/JPC0150L17-CC.pdf", "JPC0150L17-CC.pdf")</f>
         <v>JPC0150L17-CC.pdf</v>
       </c>
       <c r="C171" t="s">
@@ -6007,7 +6018,7 @@
         <v>503</v>
       </c>
       <c r="B172" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-2/EPL0490086-CC.pdf", "EPL0490086-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-2/EPL0490086-CC.pdf", "EPL0490086-CC.pdf")</f>
         <v>EPL0490086-CC.pdf</v>
       </c>
       <c r="C172" t="s">
@@ -6028,7 +6039,7 @@
         <v>506</v>
       </c>
       <c r="B173" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-2/EPL0480073-CC.pdf", "EPL0480073-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-2/EPL0480073-CC.pdf", "EPL0480073-CC.pdf")</f>
         <v>EPL0480073-CC.pdf</v>
       </c>
       <c r="C173" t="s">
@@ -6049,7 +6060,7 @@
         <v>509</v>
       </c>
       <c r="B174" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-2/JPS0710709-CC.pdf", "JPS0710709-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-2/JPS0710709-CC.pdf", "JPS0710709-CC.pdf")</f>
         <v>JPS0710709-CC.pdf</v>
       </c>
       <c r="C174" t="s">
@@ -6070,7 +6081,7 @@
         <v>512</v>
       </c>
       <c r="B175" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-2/JPS0722453-CC.pdf", "JPS0722453-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-2/JPS0722453-CC.pdf", "JPS0722453-CC.pdf")</f>
         <v>JPS0722453-CC.pdf</v>
       </c>
       <c r="C175" t="s">
@@ -6091,7 +6102,7 @@
         <v>515</v>
       </c>
       <c r="B176" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-2/JPS0731131-CC.pdf", "JPS0731131-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-2/JPS0731131-CC.pdf", "JPS0731131-CC.pdf")</f>
         <v>JPS0731131-CC.pdf</v>
       </c>
       <c r="C176" t="s">
@@ -6112,7 +6123,7 @@
         <v>518</v>
       </c>
       <c r="B177" t="str">
-        <f>HYPERLINK("http://falcon.nims.go.jp/paper_selection/documents/batch-2/JPS0731123-CC.pdf", "JPS0731123-CC.pdf")</f>
+        <f>HYPERLINK("https://github.com/lfoppiano/grobid-superconductors-data/tree/feature/material-data-validation/superconductors/corpus/pdf/batches/batch-2/JPS0731123-CC.pdf", "JPS0731123-CC.pdf")</f>
         <v>JPS0731123-CC.pdf</v>
       </c>
       <c r="C177" t="s">

</xml_diff>